<commit_message>
Se añade media, mejor y peor. Se actualiza documentacion
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/docs/flujo de caja cubiktimer.xlsx
+++ b/src/main/webapp/resources/docs/flujo de caja cubiktimer.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse_workspace\cubiktimer\src\main\webapp\resources\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cubiktimer\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,13 +13,14 @@
   </bookViews>
   <sheets>
     <sheet name="Flujo de caja" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Saldo inicial</t>
   </si>
@@ -54,9 +55,6 @@
     <t>Cobros por ventas de activo fijo</t>
   </si>
   <si>
-    <t>Pago de nómina</t>
-  </si>
-  <si>
     <t>Pago de alquiler</t>
   </si>
   <si>
@@ -69,9 +67,6 @@
     <t>Pago proveedores</t>
   </si>
   <si>
-    <t>Pago de Seguridad social</t>
-  </si>
-  <si>
     <t>Pago de servicios públicos</t>
   </si>
   <si>
@@ -94,13 +89,74 @@
   </si>
   <si>
     <t>Compra de computador</t>
+  </si>
+  <si>
+    <t>Pago de Seguridad social (Salud)</t>
+  </si>
+  <si>
+    <t>Pago de Seguridad social (Pensión)</t>
+  </si>
+  <si>
+    <t>Salario Minimo</t>
+  </si>
+  <si>
+    <t>Porcentaje Salud</t>
+  </si>
+  <si>
+    <t>Porcentaje Pension</t>
+  </si>
+  <si>
+    <t>Porcentaje parafiscales (SENA)</t>
+  </si>
+  <si>
+    <t>Porcentaje parafiscales (ICBF)</t>
+  </si>
+  <si>
+    <t>Porcentaje parafiscales (Caja de compensación)</t>
+  </si>
+  <si>
+    <t>Pago de parafiscales</t>
+  </si>
+  <si>
+    <t>Pago de Salarios</t>
+  </si>
+  <si>
+    <t>Vacaciones</t>
+  </si>
+  <si>
+    <t>Provisión Cesantías</t>
+  </si>
+  <si>
+    <t>Provisión Intereses de Cesantías</t>
+  </si>
+  <si>
+    <t>Prima de servicios</t>
+  </si>
+  <si>
+    <t>Porcentaje ARL</t>
+  </si>
+  <si>
+    <t>Provision Cesantias</t>
+  </si>
+  <si>
+    <t>Provision Intereses de cesantías</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provision vacaciones </t>
+  </si>
+  <si>
+    <t>Provision prima de servicios</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,8 +212,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,6 +250,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -232,10 +309,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -256,14 +335,32 @@
     <xf numFmtId="17" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Moneda [0]" xfId="1" builtinId="7"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="63">
+  <dxfs count="62">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -284,6 +381,14 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor rgb="FFF6FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -300,6 +405,14 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor rgb="FFF6FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -316,6 +429,14 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor rgb="FFF6FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -332,6 +453,14 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor rgb="FFF6FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -348,6 +477,14 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor rgb="FFF6FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -364,6 +501,14 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor rgb="FFF6FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -380,6 +525,14 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor rgb="FFF6FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -396,6 +549,14 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor rgb="FFF6FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -412,6 +573,14 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor rgb="FFF6FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -428,6 +597,14 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor rgb="FFF6FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -444,6 +621,14 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor rgb="FFF6FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -460,7 +645,23 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
+          <bgColor rgb="FFF6FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF6FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -476,7 +677,15 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
+          <bgColor rgb="FFF6FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -492,7 +701,15 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
+          <bgColor rgb="FFF6FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -508,7 +725,15 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
+          <bgColor rgb="FFF6FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -524,7 +749,15 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
+          <bgColor rgb="FFF6FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -540,7 +773,15 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
+          <bgColor rgb="FFF6FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -556,7 +797,15 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
+          <bgColor rgb="FFF6FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -572,7 +821,15 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
+          <bgColor rgb="FFF6FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -588,7 +845,15 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
+          <bgColor rgb="FFF6FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -604,7 +869,15 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
+          <bgColor rgb="FFF6FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -620,7 +893,15 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
+          <bgColor rgb="FFF6FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -636,7 +917,15 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
+          <bgColor rgb="FFF6FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -652,6 +941,22 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor rgb="FFF6FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF6FAFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -668,14 +973,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFF6FAFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -692,14 +989,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFF6FAFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -716,14 +1005,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFF6FAFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -740,14 +1021,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFF6FAFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -764,14 +1037,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFF6FAFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -788,14 +1053,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFF6FAFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -812,14 +1069,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFF6FAFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -836,14 +1085,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFF6FAFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -860,14 +1101,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFF6FAFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -884,14 +1117,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFF6FAFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -908,14 +1133,6 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor rgb="FFF6FAFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
           <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
@@ -927,129 +1144,6 @@
           <color theme="8"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF6FAFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF6FAFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF6FAFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF6FAFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF6FAFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF6FAFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF6FAFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF6FAFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF6FAFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF6FAFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF6FAFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF6FAFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF6FAFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF6FAFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF6FAFC"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1074,40 +1168,40 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Ingresos" displayName="Ingresos" ref="C8:N11" headerRowCount="0" totalsRowCount="1">
   <tableColumns count="12">
-    <tableColumn id="1" name="Columna1" totalsRowFunction="custom" totalsRowDxfId="11">
+    <tableColumn id="1" name="Columna1" totalsRowFunction="custom" totalsRowDxfId="61">
       <totalsRowFormula>SUM(Ingresos[Columna1])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" name="Columna2" totalsRowFunction="custom" totalsRowDxfId="10">
+    <tableColumn id="2" name="Columna2" totalsRowFunction="custom" totalsRowDxfId="60">
       <totalsRowFormula>SUM(Ingresos[Columna2])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="Columna3" totalsRowFunction="custom" totalsRowDxfId="9">
+    <tableColumn id="3" name="Columna3" totalsRowFunction="custom" totalsRowDxfId="59">
       <totalsRowFormula>SUM(Ingresos[Columna3])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="Columna4" totalsRowFunction="custom" totalsRowDxfId="8">
+    <tableColumn id="4" name="Columna4" totalsRowFunction="custom" totalsRowDxfId="58">
       <totalsRowFormula>SUM(Ingresos[Columna4])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="Columna5" totalsRowFunction="custom" totalsRowDxfId="7">
+    <tableColumn id="5" name="Columna5" totalsRowFunction="custom" totalsRowDxfId="57">
       <totalsRowFormula>SUM(Ingresos[Columna5])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="Columna6" totalsRowFunction="custom" totalsRowDxfId="6">
+    <tableColumn id="6" name="Columna6" totalsRowFunction="custom" totalsRowDxfId="56">
       <totalsRowFormula>SUM(Ingresos[Columna6])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" name="Columna7" totalsRowFunction="custom" totalsRowDxfId="5">
+    <tableColumn id="7" name="Columna7" totalsRowFunction="custom" totalsRowDxfId="55">
       <totalsRowFormula>SUM(Ingresos[Columna7])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" name="Columna8" totalsRowFunction="custom" totalsRowDxfId="4">
+    <tableColumn id="8" name="Columna8" totalsRowFunction="custom" totalsRowDxfId="54">
       <totalsRowFormula>SUM(Ingresos[Columna8])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" name="Columna9" totalsRowFunction="custom" totalsRowDxfId="3">
+    <tableColumn id="9" name="Columna9" totalsRowFunction="custom" totalsRowDxfId="53">
       <totalsRowFormula>SUM(Ingresos[Columna9])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" name="Columna10" totalsRowFunction="custom" totalsRowDxfId="2">
+    <tableColumn id="10" name="Columna10" totalsRowFunction="custom" totalsRowDxfId="52">
       <totalsRowFormula>SUM(Ingresos[Columna10])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" name="Columna11" totalsRowFunction="custom" totalsRowDxfId="1">
+    <tableColumn id="11" name="Columna11" totalsRowFunction="custom" totalsRowDxfId="51">
       <totalsRowFormula>SUM(Ingresos[Columna11])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" name="Columna12" totalsRowFunction="custom" totalsRowDxfId="0">
+    <tableColumn id="12" name="Columna12" totalsRowFunction="custom" totalsRowDxfId="50">
       <totalsRowFormula>SUM(Ingresos[Columna12])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -1116,42 +1210,42 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Egresos" displayName="Egresos" ref="C14:N23" headerRowCount="0" totalsRowCount="1" headerRowDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Egresos" displayName="Egresos" ref="C14:N29" headerRowCount="0" totalsRowCount="1" headerRowDxfId="49">
   <tableColumns count="12">
-    <tableColumn id="1" name="Columna1" totalsRowFunction="custom" headerRowDxfId="61" dataDxfId="60" totalsRowDxfId="23">
+    <tableColumn id="1" name="Columna1" totalsRowFunction="custom" headerRowDxfId="48" totalsRowDxfId="47">
       <totalsRowFormula>SUM(Egresos[Columna1])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" name="Columna2" totalsRowFunction="custom" headerRowDxfId="59" totalsRowDxfId="22">
+    <tableColumn id="2" name="Columna2" totalsRowFunction="custom" headerRowDxfId="46" totalsRowDxfId="45">
       <totalsRowFormula>SUM(Egresos[Columna2])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="Columna3" totalsRowFunction="custom" headerRowDxfId="58" totalsRowDxfId="21">
+    <tableColumn id="3" name="Columna3" totalsRowFunction="custom" headerRowDxfId="44" totalsRowDxfId="43">
       <totalsRowFormula>SUM(Egresos[Columna3])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="Columna4" totalsRowFunction="custom" headerRowDxfId="57" totalsRowDxfId="20">
+    <tableColumn id="4" name="Columna4" totalsRowFunction="custom" headerRowDxfId="42" totalsRowDxfId="41">
       <totalsRowFormula>SUM(Egresos[Columna4])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="Columna5" totalsRowFunction="custom" headerRowDxfId="56" totalsRowDxfId="19">
+    <tableColumn id="5" name="Columna5" totalsRowFunction="custom" headerRowDxfId="40" totalsRowDxfId="39">
       <totalsRowFormula>SUM(Egresos[Columna5])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="Columna6" totalsRowFunction="custom" headerRowDxfId="55" totalsRowDxfId="18">
+    <tableColumn id="6" name="Columna6" totalsRowFunction="custom" headerRowDxfId="38" totalsRowDxfId="37">
       <totalsRowFormula>SUM(Egresos[Columna6])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" name="Columna7" totalsRowFunction="custom" headerRowDxfId="54" totalsRowDxfId="17">
+    <tableColumn id="7" name="Columna7" totalsRowFunction="custom" headerRowDxfId="36" totalsRowDxfId="35">
       <totalsRowFormula>SUM(Egresos[Columna7])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" name="Columna8" totalsRowFunction="custom" headerRowDxfId="53" totalsRowDxfId="16">
+    <tableColumn id="8" name="Columna8" totalsRowFunction="custom" headerRowDxfId="34" totalsRowDxfId="33">
       <totalsRowFormula>SUM(Egresos[Columna8])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" name="Columna9" totalsRowFunction="custom" headerRowDxfId="52" totalsRowDxfId="15">
+    <tableColumn id="9" name="Columna9" totalsRowFunction="custom" headerRowDxfId="32" totalsRowDxfId="31">
       <totalsRowFormula>SUM(Egresos[Columna9])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" name="Columna10" totalsRowFunction="custom" headerRowDxfId="51" totalsRowDxfId="14">
+    <tableColumn id="10" name="Columna10" totalsRowFunction="custom" headerRowDxfId="30" totalsRowDxfId="29">
       <totalsRowFormula>SUM(Egresos[Columna10])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" name="Columna11" totalsRowFunction="custom" headerRowDxfId="50" totalsRowDxfId="13">
+    <tableColumn id="11" name="Columna11" totalsRowFunction="custom" headerRowDxfId="28" totalsRowDxfId="27">
       <totalsRowFormula>SUM(Egresos[Columna11])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" name="Columna12" totalsRowFunction="custom" headerRowDxfId="49" totalsRowDxfId="12">
+    <tableColumn id="12" name="Columna12" totalsRowFunction="custom" headerRowDxfId="26" totalsRowDxfId="25">
       <totalsRowFormula>SUM(Egresos[Columna12])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -1160,42 +1254,42 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Financiamiento" displayName="Financiamiento" ref="C28:N30" headerRowCount="0" totalsRowCount="1" headerRowDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Financiamiento" displayName="Financiamiento" ref="C34:N36" headerRowCount="0" totalsRowCount="1" headerRowDxfId="24">
   <tableColumns count="12">
-    <tableColumn id="1" name="Columna1" totalsRowFunction="custom" headerRowDxfId="47" totalsRowDxfId="46">
+    <tableColumn id="1" name="Columna1" totalsRowFunction="custom" headerRowDxfId="23" totalsRowDxfId="22">
       <totalsRowFormula>SUM(Financiamiento[Columna1])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" name="Columna2" totalsRowFunction="custom" headerRowDxfId="45" totalsRowDxfId="44">
+    <tableColumn id="2" name="Columna2" totalsRowFunction="custom" headerRowDxfId="21" totalsRowDxfId="20">
       <totalsRowFormula>SUM(Financiamiento[Columna2])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" name="Columna3" totalsRowFunction="custom" headerRowDxfId="43" totalsRowDxfId="42">
+    <tableColumn id="3" name="Columna3" totalsRowFunction="custom" headerRowDxfId="19" totalsRowDxfId="18">
       <totalsRowFormula>SUM(Financiamiento[Columna3])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="4" name="Columna4" totalsRowFunction="custom" headerRowDxfId="41" totalsRowDxfId="40">
+    <tableColumn id="4" name="Columna4" totalsRowFunction="custom" headerRowDxfId="17" totalsRowDxfId="16">
       <totalsRowFormula>SUM(Financiamiento[Columna4])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="Columna5" totalsRowFunction="custom" headerRowDxfId="39" totalsRowDxfId="38">
+    <tableColumn id="5" name="Columna5" totalsRowFunction="custom" headerRowDxfId="15" totalsRowDxfId="14">
       <totalsRowFormula>SUM(Financiamiento[Columna5])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="Columna6" totalsRowFunction="custom" headerRowDxfId="37" totalsRowDxfId="36">
+    <tableColumn id="6" name="Columna6" totalsRowFunction="custom" headerRowDxfId="13" totalsRowDxfId="12">
       <totalsRowFormula>SUM(Financiamiento[Columna6])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" name="Columna7" totalsRowFunction="custom" headerRowDxfId="35" totalsRowDxfId="34">
+    <tableColumn id="7" name="Columna7" totalsRowFunction="custom" headerRowDxfId="11" totalsRowDxfId="10">
       <totalsRowFormula>SUM(Financiamiento[Columna7])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="8" name="Columna8" totalsRowFunction="custom" headerRowDxfId="33" totalsRowDxfId="32">
+    <tableColumn id="8" name="Columna8" totalsRowFunction="custom" headerRowDxfId="9" totalsRowDxfId="8">
       <totalsRowFormula>SUM(Financiamiento[Columna8])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="9" name="Columna9" totalsRowFunction="custom" headerRowDxfId="31" totalsRowDxfId="30">
+    <tableColumn id="9" name="Columna9" totalsRowFunction="custom" headerRowDxfId="7" totalsRowDxfId="6">
       <totalsRowFormula>SUM(Financiamiento[Columna9])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="10" name="Columna10" totalsRowFunction="custom" headerRowDxfId="29" totalsRowDxfId="28">
+    <tableColumn id="10" name="Columna10" totalsRowFunction="custom" headerRowDxfId="5" totalsRowDxfId="4">
       <totalsRowFormula>SUM(Financiamiento[Columna10])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="11" name="Columna11" totalsRowFunction="custom" headerRowDxfId="27" totalsRowDxfId="26">
+    <tableColumn id="11" name="Columna11" totalsRowFunction="custom" headerRowDxfId="3" totalsRowDxfId="2">
       <totalsRowFormula>SUM(Financiamiento[Columna11])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="12" name="Columna12" totalsRowFunction="custom" headerRowDxfId="25" totalsRowDxfId="24">
+    <tableColumn id="12" name="Columna12" totalsRowFunction="custom" headerRowDxfId="1" totalsRowDxfId="0">
       <totalsRowFormula>SUM(Financiamiento[Columna12])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -1490,17 +1584,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:O32"/>
+  <dimension ref="B1:O38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
@@ -1511,28 +1605,28 @@
     <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="35.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
     </row>
     <row r="2" spans="2:15" ht="16.5" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:15" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -1583,48 +1677,48 @@
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1">
-        <f>C32</f>
-        <v>1850000</v>
+        <f>C38</f>
+        <v>6280237</v>
       </c>
       <c r="E5" s="1">
-        <f>D32</f>
-        <v>2280000</v>
+        <f>D38</f>
+        <v>5448343.3899999997</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" ref="F5:N5" si="0">E32</f>
-        <v>2110000</v>
+        <f t="shared" ref="F5:N5" si="0">E38</f>
+        <v>3800974.3899999997</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>2420000</v>
+        <v>2812084.78</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="0"/>
-        <v>2160000</v>
+        <v>11018518.779999999</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="0"/>
-        <v>1690000</v>
+        <v>8907159.7799999993</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="0"/>
-        <v>1690000</v>
+        <v>7194391.7799999993</v>
       </c>
       <c r="K5" s="1">
         <f t="shared" si="0"/>
-        <v>1690000</v>
+        <v>5481623.7799999993</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="0"/>
-        <v>1690000</v>
+        <v>13768855.779999999</v>
       </c>
       <c r="M5" s="1">
         <f t="shared" si="0"/>
-        <v>1690000</v>
+        <v>12056087.779999999</v>
       </c>
       <c r="N5" s="1">
         <f t="shared" si="0"/>
-        <v>1690000</v>
+        <v>10343319.779999999</v>
       </c>
       <c r="O5" s="1"/>
     </row>
@@ -1648,25 +1742,25 @@
     </row>
     <row r="8" spans="2:15" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8">
-        <v>5000000</v>
+        <v>10000000</v>
       </c>
       <c r="D8">
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>1000000</v>
+        <v>10000000</v>
       </c>
       <c r="H8">
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -1675,7 +1769,7 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>10000000</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -1688,7 +1782,7 @@
       </c>
       <c r="O8">
         <f>SUM(Ingresos[[#This Row],[Columna1]:[Columna12]])</f>
-        <v>10000000</v>
+        <v>30000000</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="15" x14ac:dyDescent="0.25">
@@ -1783,31 +1877,31 @@
     </row>
     <row r="11" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1">
         <f>SUM(Ingresos[Columna1])</f>
-        <v>5000000</v>
+        <v>10000000</v>
       </c>
       <c r="D11" s="1">
         <f>SUM(Ingresos[Columna2])</f>
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="E11" s="1">
         <f>SUM(Ingresos[Columna3])</f>
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="F11" s="1">
         <f>SUM(Ingresos[Columna4])</f>
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="G11" s="1">
         <f>SUM(Ingresos[Columna5])</f>
-        <v>1000000</v>
+        <v>10000000</v>
       </c>
       <c r="H11" s="1">
         <f>SUM(Ingresos[Columna6])</f>
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="I11" s="1">
         <f>SUM(Ingresos[Columna7])</f>
@@ -1819,7 +1913,7 @@
       </c>
       <c r="K11" s="1">
         <f>SUM(Ingresos[Columna9])</f>
-        <v>0</v>
+        <v>10000000</v>
       </c>
       <c r="L11" s="1">
         <f>SUM(Ingresos[Columna10])</f>
@@ -1835,7 +1929,7 @@
       </c>
       <c r="O11" s="1">
         <f>SUM(Ingresos[#Totals])</f>
-        <v>10000000</v>
+        <v>30000000</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
@@ -1858,7 +1952,7 @@
     </row>
     <row r="14" spans="2:15" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14">
         <v>1800000</v>
@@ -1902,697 +1996,1051 @@
       </c>
     </row>
     <row r="15" spans="2:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="25">
+        <v>1110000</v>
+      </c>
+      <c r="D15" s="25">
+        <v>330000</v>
+      </c>
+      <c r="E15" s="25">
+        <v>930000</v>
+      </c>
+      <c r="F15" s="25">
+        <v>450000</v>
+      </c>
+      <c r="G15" s="25">
+        <v>1020000</v>
+      </c>
+      <c r="H15" s="25">
+        <v>1230000</v>
+      </c>
+      <c r="I15" s="25">
+        <v>960000</v>
+      </c>
+      <c r="J15" s="25">
+        <v>960000</v>
+      </c>
+      <c r="K15" s="25">
+        <v>960000</v>
+      </c>
+      <c r="L15" s="25">
+        <v>960000</v>
+      </c>
+      <c r="M15" s="25">
+        <v>960000</v>
+      </c>
+      <c r="N15" s="25">
+        <v>960000</v>
+      </c>
+      <c r="O15" s="25">
+        <f>SUM(Egresos[[#This Row],[Columna1]:[Columna12]])</f>
+        <v>10830000</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B16" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="25">
+        <f>IF(C15&lt;Hoja1!$B$2,Hoja1!$B$2*Hoja1!$B$3,'Flujo de caja'!C15*Hoja1!$B$3)</f>
+        <v>94350</v>
+      </c>
+      <c r="D16" s="25">
+        <f>IF(D15&lt;Hoja1!$B$2,Hoja1!$B$2*Hoja1!$B$3,'Flujo de caja'!D15*Hoja1!$B$3)</f>
+        <v>66405.570000000007</v>
+      </c>
+      <c r="E16" s="25">
+        <f>IF(E15&lt;Hoja1!$B$2,Hoja1!$B$2*Hoja1!$B$3,'Flujo de caja'!E15*Hoja1!$B$3)</f>
+        <v>79050</v>
+      </c>
+      <c r="F16" s="25">
+        <f>IF(F15&lt;Hoja1!$B$2,Hoja1!$B$2*Hoja1!$B$3,'Flujo de caja'!F15*Hoja1!$B$3)</f>
+        <v>66405.570000000007</v>
+      </c>
+      <c r="G16" s="25">
+        <f>IF(G15&lt;Hoja1!$C$2,Hoja1!$C$2*Hoja1!$C$3,'Flujo de caja'!G15*Hoja1!$C$3)</f>
+        <v>86700</v>
+      </c>
+      <c r="H16" s="25">
+        <f>IF(H15&lt;Hoja1!$C$2,Hoja1!$C$2*Hoja1!$C$3,'Flujo de caja'!H15*Hoja1!$C$3)</f>
+        <v>104550.00000000001</v>
+      </c>
+      <c r="I16" s="25">
+        <f>IF(I15&lt;Hoja1!$C$2,Hoja1!$C$2*Hoja1!$C$3,'Flujo de caja'!I15*Hoja1!$C$3)</f>
+        <v>81600</v>
+      </c>
+      <c r="J16" s="25">
+        <f>IF(J15&lt;Hoja1!$C$2,Hoja1!$C$2*Hoja1!$C$3,'Flujo de caja'!J15*Hoja1!$C$3)</f>
+        <v>81600</v>
+      </c>
+      <c r="K16" s="25">
+        <f>IF(K15&lt;Hoja1!$C$2,Hoja1!$C$2*Hoja1!$C$3,'Flujo de caja'!K15*Hoja1!$C$3)</f>
+        <v>81600</v>
+      </c>
+      <c r="L16" s="25">
+        <f>IF(L15&lt;Hoja1!$C$2,Hoja1!$C$2*Hoja1!$C$3,'Flujo de caja'!L15*Hoja1!$C$3)</f>
+        <v>81600</v>
+      </c>
+      <c r="M16" s="25">
+        <f>IF(M15&lt;Hoja1!$C$2,Hoja1!$C$2*Hoja1!$C$3,'Flujo de caja'!M15*Hoja1!$C$3)</f>
+        <v>81600</v>
+      </c>
+      <c r="N16" s="25">
+        <f>IF(N15&lt;Hoja1!$C$2,Hoja1!$C$2*Hoja1!$C$3,'Flujo de caja'!N15*Hoja1!$C$3)</f>
+        <v>81600</v>
+      </c>
+      <c r="O16" s="25">
+        <f>SUM(Egresos[[#This Row],[Columna1]:[Columna12]])</f>
+        <v>987061.14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B17" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="25">
+        <f>IF(C15&lt;Hoja1!$B$2,Hoja1!$B$2*Hoja1!$B$4,'Flujo de caja'!C15*Hoja1!$B$4)</f>
+        <v>133200</v>
+      </c>
+      <c r="D17" s="25">
+        <f>IF(D15&lt;Hoja1!$B$2,Hoja1!$B$2*Hoja1!$B$4,'Flujo de caja'!D15*Hoja1!$B$4)</f>
+        <v>93749.04</v>
+      </c>
+      <c r="E17" s="25">
+        <f>IF(E15&lt;Hoja1!$B$2,Hoja1!$B$2*Hoja1!$B$4,'Flujo de caja'!E15*Hoja1!$B$4)</f>
+        <v>111600</v>
+      </c>
+      <c r="F17" s="25">
+        <f>IF(F15&lt;Hoja1!$B$2,Hoja1!$B$2*Hoja1!$B$4,'Flujo de caja'!F15*Hoja1!$B$4)</f>
+        <v>93749.04</v>
+      </c>
+      <c r="G17" s="25">
+        <f>IF(G15&lt;Hoja1!$C$2,Hoja1!$C$2*Hoja1!$C$4,'Flujo de caja'!G15*Hoja1!$C$4)</f>
+        <v>122400</v>
+      </c>
+      <c r="H17" s="25">
+        <f>IF(H15&lt;Hoja1!$C$2,Hoja1!$C$2*Hoja1!$C$4,'Flujo de caja'!H15*Hoja1!$C$4)</f>
+        <v>147600</v>
+      </c>
+      <c r="I17" s="25">
+        <f>IF(I15&lt;Hoja1!$C$2,Hoja1!$C$2*Hoja1!$C$4,'Flujo de caja'!I15*Hoja1!$C$4)</f>
+        <v>115200</v>
+      </c>
+      <c r="J17" s="25">
+        <f>IF(J15&lt;Hoja1!$C$2,Hoja1!$C$2*Hoja1!$C$4,'Flujo de caja'!J15*Hoja1!$C$4)</f>
+        <v>115200</v>
+      </c>
+      <c r="K17" s="25">
+        <f>IF(K15&lt;Hoja1!$C$2,Hoja1!$C$2*Hoja1!$C$4,'Flujo de caja'!K15*Hoja1!$C$4)</f>
+        <v>115200</v>
+      </c>
+      <c r="L17" s="25">
+        <f>IF(L15&lt;Hoja1!$C$2,Hoja1!$C$2*Hoja1!$C$4,'Flujo de caja'!L15*Hoja1!$C$4)</f>
+        <v>115200</v>
+      </c>
+      <c r="M17" s="25">
+        <f>IF(M15&lt;Hoja1!$C$2,Hoja1!$C$2*Hoja1!$C$4,'Flujo de caja'!M15*Hoja1!$C$4)</f>
+        <v>115200</v>
+      </c>
+      <c r="N17" s="25">
+        <f>IF(N15&lt;Hoja1!$C$2,Hoja1!$C$2*Hoja1!$C$4,'Flujo de caja'!N15*Hoja1!$C$4)</f>
+        <v>115200</v>
+      </c>
+      <c r="O17" s="25">
+        <f>SUM(Egresos[[#This Row],[Columna1]:[Columna12]])</f>
+        <v>1393498.08</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B18" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="25">
+        <f>C15*SUM(Hoja1!$B$5:$B$7)</f>
+        <v>99900</v>
+      </c>
+      <c r="D18" s="25">
+        <f>D15*SUM(Hoja1!$B$5:$B$7)</f>
+        <v>29700</v>
+      </c>
+      <c r="E18" s="25">
+        <f>E15*SUM(Hoja1!$B$5:$B$7)</f>
+        <v>83700</v>
+      </c>
+      <c r="F18" s="25">
+        <f>F15*SUM(Hoja1!$B$5:$B$7)</f>
+        <v>40500</v>
+      </c>
+      <c r="G18" s="25">
+        <f>G15*SUM(Hoja1!$C$5:$C$7)</f>
+        <v>91800</v>
+      </c>
+      <c r="H18" s="25">
+        <f>H15*SUM(Hoja1!$C$5:$C$7)</f>
+        <v>110700</v>
+      </c>
+      <c r="I18" s="25">
+        <f>I15*SUM(Hoja1!$C$5:$C$7)</f>
+        <v>86400</v>
+      </c>
+      <c r="J18" s="25">
+        <f>J15*SUM(Hoja1!$C$5:$C$7)</f>
+        <v>86400</v>
+      </c>
+      <c r="K18" s="25">
+        <f>K15*SUM(Hoja1!$C$5:$C$7)</f>
+        <v>86400</v>
+      </c>
+      <c r="L18" s="25">
+        <f>L15*SUM(Hoja1!$C$5:$C$7)</f>
+        <v>86400</v>
+      </c>
+      <c r="M18" s="25">
+        <f>M15*SUM(Hoja1!$C$5:$C$7)</f>
+        <v>86400</v>
+      </c>
+      <c r="N18" s="25">
+        <f>N15*SUM(Hoja1!$C$5:$C$7)</f>
+        <v>86400</v>
+      </c>
+      <c r="O18" s="25">
+        <f>O15*SUM(Hoja1!$C$5:$C$7)</f>
+        <v>974700</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B19" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="25">
+        <f>C$15*Hoja1!$B8</f>
+        <v>92463</v>
+      </c>
+      <c r="D19" s="25">
+        <f>D$15*Hoja1!$B8</f>
+        <v>27489</v>
+      </c>
+      <c r="E19" s="25">
+        <f>E$15*Hoja1!$B8</f>
+        <v>77469</v>
+      </c>
+      <c r="F19" s="25">
+        <f>F$15*Hoja1!$B8</f>
+        <v>37485</v>
+      </c>
+      <c r="G19" s="25">
+        <f>G$15*Hoja1!$C8</f>
+        <v>84966</v>
+      </c>
+      <c r="H19" s="25">
+        <f>H$15*Hoja1!$C8</f>
+        <v>102459</v>
+      </c>
+      <c r="I19" s="25">
+        <f>I$15*Hoja1!$C8</f>
+        <v>79968</v>
+      </c>
+      <c r="J19" s="25">
+        <f>J$15*Hoja1!$C8</f>
+        <v>79968</v>
+      </c>
+      <c r="K19" s="25">
+        <f>K$15*Hoja1!$C8</f>
+        <v>79968</v>
+      </c>
+      <c r="L19" s="25">
+        <f>L$15*Hoja1!$C8</f>
+        <v>79968</v>
+      </c>
+      <c r="M19" s="25">
+        <f>M$15*Hoja1!$C8</f>
+        <v>79968</v>
+      </c>
+      <c r="N19" s="25">
+        <f>N$15*Hoja1!$C8</f>
+        <v>79968</v>
+      </c>
+      <c r="O19" s="25">
+        <f>O$15*Hoja1!$C8</f>
+        <v>902139</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B20" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="25">
+        <f>C$15*Hoja1!$B9</f>
+        <v>11100</v>
+      </c>
+      <c r="D20" s="25">
+        <f>D$15*Hoja1!$B9</f>
+        <v>3300</v>
+      </c>
+      <c r="E20" s="25">
+        <f>E$15*Hoja1!$B9</f>
+        <v>9300</v>
+      </c>
+      <c r="F20" s="25">
+        <f>F$15*Hoja1!$B9</f>
+        <v>4500</v>
+      </c>
+      <c r="G20" s="25">
+        <f>G$15*Hoja1!$C9</f>
+        <v>10200</v>
+      </c>
+      <c r="H20" s="25">
+        <f>H$15*Hoja1!$C9</f>
+        <v>12300</v>
+      </c>
+      <c r="I20" s="25">
+        <f>I$15*Hoja1!$C9</f>
+        <v>9600</v>
+      </c>
+      <c r="J20" s="25">
+        <f>J$15*Hoja1!$C9</f>
+        <v>9600</v>
+      </c>
+      <c r="K20" s="25">
+        <f>K$15*Hoja1!$C9</f>
+        <v>9600</v>
+      </c>
+      <c r="L20" s="25">
+        <f>L$15*Hoja1!$C9</f>
+        <v>9600</v>
+      </c>
+      <c r="M20" s="25">
+        <f>M$15*Hoja1!$C9</f>
+        <v>9600</v>
+      </c>
+      <c r="N20" s="25">
+        <f>N$15*Hoja1!$C9</f>
+        <v>9600</v>
+      </c>
+      <c r="O20" s="25">
+        <f>O$15*Hoja1!$C9</f>
+        <v>108300</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B21" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="25">
+        <f>C$15*Hoja1!$B10</f>
+        <v>92463</v>
+      </c>
+      <c r="D21" s="25">
+        <f>D$15*Hoja1!$B10</f>
+        <v>27489</v>
+      </c>
+      <c r="E21" s="25">
+        <f>E$15*Hoja1!$B10</f>
+        <v>77469</v>
+      </c>
+      <c r="F21" s="25">
+        <f>F$15*Hoja1!$B10</f>
+        <v>37485</v>
+      </c>
+      <c r="G21" s="25">
+        <f>G$15*Hoja1!$C10</f>
+        <v>84966</v>
+      </c>
+      <c r="H21" s="25">
+        <f>H$15*Hoja1!$C10</f>
+        <v>102459</v>
+      </c>
+      <c r="I21" s="25">
+        <f>I$15*Hoja1!$C10</f>
+        <v>79968</v>
+      </c>
+      <c r="J21" s="25">
+        <f>J$15*Hoja1!$C10</f>
+        <v>79968</v>
+      </c>
+      <c r="K21" s="25">
+        <f>K$15*Hoja1!$C10</f>
+        <v>79968</v>
+      </c>
+      <c r="L21" s="25">
+        <f>L$15*Hoja1!$C10</f>
+        <v>79968</v>
+      </c>
+      <c r="M21" s="25">
+        <f>M$15*Hoja1!$C10</f>
+        <v>79968</v>
+      </c>
+      <c r="N21" s="25">
+        <f>N$15*Hoja1!$C10</f>
+        <v>79968</v>
+      </c>
+      <c r="O21" s="25">
+        <f>O$15*Hoja1!$C10</f>
+        <v>902139</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B22" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="25">
+        <f>C$15*Hoja1!$B11</f>
+        <v>46287</v>
+      </c>
+      <c r="D22" s="25">
+        <f>D$15*Hoja1!$B11</f>
+        <v>13761</v>
+      </c>
+      <c r="E22" s="25">
+        <f>E$15*Hoja1!$B11</f>
+        <v>38781</v>
+      </c>
+      <c r="F22" s="25">
+        <f>F$15*Hoja1!$B11</f>
+        <v>18765</v>
+      </c>
+      <c r="G22" s="25">
+        <f>G$15*Hoja1!$C11</f>
+        <v>42534</v>
+      </c>
+      <c r="H22" s="25">
+        <f>H$15*Hoja1!$C11</f>
+        <v>51291</v>
+      </c>
+      <c r="I22" s="25">
+        <f>I$15*Hoja1!$C11</f>
+        <v>40032</v>
+      </c>
+      <c r="J22" s="25">
+        <f>J$15*Hoja1!$C11</f>
+        <v>40032</v>
+      </c>
+      <c r="K22" s="25">
+        <f>K$15*Hoja1!$C11</f>
+        <v>40032</v>
+      </c>
+      <c r="L22" s="25">
+        <f>L$15*Hoja1!$C11</f>
+        <v>40032</v>
+      </c>
+      <c r="M22" s="25">
+        <f>M$15*Hoja1!$C11</f>
+        <v>40032</v>
+      </c>
+      <c r="N22" s="25">
+        <f>N$15*Hoja1!$C11</f>
+        <v>40032</v>
+      </c>
+      <c r="O22" s="25">
+        <f>O$15*Hoja1!$C11</f>
+        <v>451611</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <f>SUM(Egresos[[#This Row],[Columna1]:[Columna12]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B24" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <f>SUM(Egresos[[#This Row],[Columna1]:[Columna12]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B25" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25">
+        <v>140000</v>
+      </c>
+      <c r="D25">
+        <v>140000</v>
+      </c>
+      <c r="E25">
+        <v>140000</v>
+      </c>
+      <c r="F25">
+        <v>140000</v>
+      </c>
+      <c r="G25">
+        <v>140000</v>
+      </c>
+      <c r="H25">
+        <v>140000</v>
+      </c>
+      <c r="I25">
+        <v>150000</v>
+      </c>
+      <c r="J25">
+        <v>150000</v>
+      </c>
+      <c r="K25">
+        <v>150000</v>
+      </c>
+      <c r="L25">
+        <v>150000</v>
+      </c>
+      <c r="M25">
+        <v>150000</v>
+      </c>
+      <c r="N25">
+        <v>150000</v>
+      </c>
+      <c r="O25">
+        <f>SUM(Egresos[[#This Row],[Columna1]:[Columna12]])</f>
+        <v>1740000</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B26" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C15">
-        <v>1110000</v>
-      </c>
-      <c r="D15">
-        <v>330000</v>
-      </c>
-      <c r="E15">
-        <v>930000</v>
-      </c>
-      <c r="F15">
-        <v>450000</v>
-      </c>
-      <c r="G15">
-        <v>1020000</v>
-      </c>
-      <c r="H15">
-        <v>1230000</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15">
+      <c r="C26">
+        <v>100000</v>
+      </c>
+      <c r="D26">
+        <v>100000</v>
+      </c>
+      <c r="E26">
+        <v>100000</v>
+      </c>
+      <c r="F26">
+        <v>100000</v>
+      </c>
+      <c r="G26">
+        <v>110000</v>
+      </c>
+      <c r="H26">
+        <v>110000</v>
+      </c>
+      <c r="I26">
+        <v>110000</v>
+      </c>
+      <c r="J26">
+        <v>110000</v>
+      </c>
+      <c r="K26">
+        <v>110000</v>
+      </c>
+      <c r="L26">
+        <v>110000</v>
+      </c>
+      <c r="M26">
+        <v>110000</v>
+      </c>
+      <c r="N26">
+        <v>110000</v>
+      </c>
+      <c r="O26">
         <f>SUM(Egresos[[#This Row],[Columna1]:[Columna12]])</f>
-        <v>5070000</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B16" s="8" t="s">
+        <v>1280000</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16">
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
         <f>SUM(Egresos[[#This Row],[Columna1]:[Columna12]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="2:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B17" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17">
-        <f>SUM(Egresos[[#This Row],[Columna1]:[Columna12]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B18" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-      <c r="O18">
-        <f>SUM(Egresos[[#This Row],[Columna1]:[Columna12]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B19" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19">
-        <v>140000</v>
-      </c>
-      <c r="D19">
-        <v>140000</v>
-      </c>
-      <c r="E19">
-        <v>140000</v>
-      </c>
-      <c r="F19">
-        <v>140000</v>
-      </c>
-      <c r="G19">
-        <v>140000</v>
-      </c>
-      <c r="H19">
-        <v>140000</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="O19">
-        <f>SUM(Egresos[[#This Row],[Columna1]:[Columna12]])</f>
-        <v>840000</v>
-      </c>
-    </row>
-    <row r="20" spans="2:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B20" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20">
-        <v>100000</v>
-      </c>
-      <c r="D20">
-        <v>100000</v>
-      </c>
-      <c r="E20">
-        <v>100000</v>
-      </c>
-      <c r="F20">
-        <v>100000</v>
-      </c>
-      <c r="G20">
-        <v>100000</v>
-      </c>
-      <c r="H20">
-        <v>100000</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20">
-        <f>SUM(Egresos[[#This Row],[Columna1]:[Columna12]])</f>
-        <v>600000</v>
-      </c>
-    </row>
-    <row r="21" spans="2:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B21" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
-      <c r="O21">
-        <f>SUM(Egresos[[#This Row],[Columna1]:[Columna12]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B22" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <v>0</v>
-      </c>
-      <c r="O22">
-        <f>SUM(Egresos[[#This Row],[Columna1]:[Columna12]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="1">
-        <f>SUM(Egresos[Columna1])</f>
-        <v>3150000</v>
-      </c>
-      <c r="D23" s="1">
-        <f>SUM(Egresos[Columna2])</f>
-        <v>570000</v>
-      </c>
-      <c r="E23" s="1">
-        <f>SUM(Egresos[Columna3])</f>
-        <v>1170000</v>
-      </c>
-      <c r="F23" s="1">
-        <f>SUM(Egresos[Columna4])</f>
-        <v>690000</v>
-      </c>
-      <c r="G23" s="1">
-        <f>SUM(Egresos[Columna5])</f>
-        <v>1260000</v>
-      </c>
-      <c r="H23" s="1">
-        <f>SUM(Egresos[Columna6])</f>
-        <v>1470000</v>
-      </c>
-      <c r="I23" s="1">
-        <f>SUM(Egresos[Columna7])</f>
-        <v>0</v>
-      </c>
-      <c r="J23" s="1">
-        <f>SUM(Egresos[Columna8])</f>
-        <v>0</v>
-      </c>
-      <c r="K23" s="1">
-        <f>SUM(Egresos[Columna9])</f>
-        <v>0</v>
-      </c>
-      <c r="L23" s="1">
-        <f>SUM(Egresos[Columna10])</f>
-        <v>0</v>
-      </c>
-      <c r="M23" s="1">
-        <f>SUM(Egresos[Columna11])</f>
-        <v>0</v>
-      </c>
-      <c r="N23" s="1">
-        <f>SUM(Egresos[Columna12])</f>
-        <v>0</v>
-      </c>
-      <c r="O23" s="1">
-        <f>SUM(Egresos[#Totals])</f>
-        <v>8310000</v>
-      </c>
-    </row>
-    <row r="24" spans="2:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B24" s="3"/>
-    </row>
-    <row r="25" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="10">
-        <f>C5+Ingresos[[#Totals],[Columna1]]-Egresos[[#Totals],[Columna1]]</f>
-        <v>1850000</v>
-      </c>
-      <c r="D25" s="10">
-        <f>D5+Ingresos[[#Totals],[Columna2]]-Egresos[[#Totals],[Columna2]]</f>
-        <v>2280000</v>
-      </c>
-      <c r="E25" s="10">
-        <f>E5+Ingresos[[#Totals],[Columna3]]-Egresos[[#Totals],[Columna3]]</f>
-        <v>2110000</v>
-      </c>
-      <c r="F25" s="10">
-        <f>F5+Ingresos[[#Totals],[Columna4]]-Egresos[[#Totals],[Columna4]]</f>
-        <v>2420000</v>
-      </c>
-      <c r="G25" s="10">
-        <f>G5+Ingresos[[#Totals],[Columna5]]-Egresos[[#Totals],[Columna5]]</f>
-        <v>2160000</v>
-      </c>
-      <c r="H25" s="10">
-        <f>H5+Ingresos[[#Totals],[Columna6]]-Egresos[[#Totals],[Columna6]]</f>
-        <v>1690000</v>
-      </c>
-      <c r="I25" s="10">
-        <f>I5+Ingresos[[#Totals],[Columna7]]-Egresos[[#Totals],[Columna7]]</f>
-        <v>1690000</v>
-      </c>
-      <c r="J25" s="10">
-        <f>J5+Ingresos[[#Totals],[Columna8]]-Egresos[[#Totals],[Columna8]]</f>
-        <v>1690000</v>
-      </c>
-      <c r="K25" s="10">
-        <f>K5+Ingresos[[#Totals],[Columna9]]-Egresos[[#Totals],[Columna9]]</f>
-        <v>1690000</v>
-      </c>
-      <c r="L25" s="10">
-        <f>L5+Ingresos[[#Totals],[Columna10]]-Egresos[[#Totals],[Columna10]]</f>
-        <v>1690000</v>
-      </c>
-      <c r="M25" s="10">
-        <f>M5+Ingresos[[#Totals],[Columna11]]-Egresos[[#Totals],[Columna11]]</f>
-        <v>1690000</v>
-      </c>
-      <c r="N25" s="10">
-        <f>N5+Ingresos[[#Totals],[Columna12]]-Egresos[[#Totals],[Columna12]]</f>
-        <v>1690000</v>
-      </c>
-      <c r="O25" s="10"/>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B27" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
     </row>
     <row r="28" spans="2:15" ht="15" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <f>SUM(Egresos[[#This Row],[Columna1]:[Columna12]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="1">
+        <f>SUM(Egresos[Columna1])</f>
+        <v>3719763</v>
+      </c>
+      <c r="D29" s="1">
+        <f>SUM(Egresos[Columna2])</f>
+        <v>831893.61</v>
+      </c>
+      <c r="E29" s="1">
+        <f>SUM(Egresos[Columna3])</f>
+        <v>1647369</v>
+      </c>
+      <c r="F29" s="1">
+        <f>SUM(Egresos[Columna4])</f>
+        <v>988889.61</v>
+      </c>
+      <c r="G29" s="1">
+        <f>SUM(Egresos[Columna5])</f>
+        <v>1793566</v>
+      </c>
+      <c r="H29" s="1">
+        <f>SUM(Egresos[Columna6])</f>
+        <v>2111359</v>
+      </c>
+      <c r="I29" s="1">
+        <f>SUM(Egresos[Columna7])</f>
+        <v>1712768</v>
+      </c>
+      <c r="J29" s="1">
+        <f>SUM(Egresos[Columna8])</f>
+        <v>1712768</v>
+      </c>
+      <c r="K29" s="1">
+        <f>SUM(Egresos[Columna9])</f>
+        <v>1712768</v>
+      </c>
+      <c r="L29" s="1">
+        <f>SUM(Egresos[Columna10])</f>
+        <v>1712768</v>
+      </c>
+      <c r="M29" s="1">
+        <f>SUM(Egresos[Columna11])</f>
+        <v>1712768</v>
+      </c>
+      <c r="N29" s="1">
+        <f>SUM(Egresos[Columna12])</f>
+        <v>1712768</v>
+      </c>
+      <c r="O29" s="1">
+        <f>SUM(Egresos[#Totals])</f>
+        <v>21369448.219999999</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="10">
+        <f>C5+Ingresos[[#Totals],[Columna1]]-Egresos[[#Totals],[Columna1]]</f>
+        <v>6280237</v>
+      </c>
+      <c r="D31" s="10">
+        <f>D5+Ingresos[[#Totals],[Columna2]]-Egresos[[#Totals],[Columna2]]</f>
+        <v>5448343.3899999997</v>
+      </c>
+      <c r="E31" s="10">
+        <f>E5+Ingresos[[#Totals],[Columna3]]-Egresos[[#Totals],[Columna3]]</f>
+        <v>3800974.3899999997</v>
+      </c>
+      <c r="F31" s="10">
+        <f>F5+Ingresos[[#Totals],[Columna4]]-Egresos[[#Totals],[Columna4]]</f>
+        <v>2812084.78</v>
+      </c>
+      <c r="G31" s="10">
+        <f>G5+Ingresos[[#Totals],[Columna5]]-Egresos[[#Totals],[Columna5]]</f>
+        <v>11018518.779999999</v>
+      </c>
+      <c r="H31" s="10">
+        <f>H5+Ingresos[[#Totals],[Columna6]]-Egresos[[#Totals],[Columna6]]</f>
+        <v>8907159.7799999993</v>
+      </c>
+      <c r="I31" s="10">
+        <f>I5+Ingresos[[#Totals],[Columna7]]-Egresos[[#Totals],[Columna7]]</f>
+        <v>7194391.7799999993</v>
+      </c>
+      <c r="J31" s="10">
+        <f>J5+Ingresos[[#Totals],[Columna8]]-Egresos[[#Totals],[Columna8]]</f>
+        <v>5481623.7799999993</v>
+      </c>
+      <c r="K31" s="10">
+        <f>K5+Ingresos[[#Totals],[Columna9]]-Egresos[[#Totals],[Columna9]]</f>
+        <v>13768855.779999999</v>
+      </c>
+      <c r="L31" s="10">
+        <f>L5+Ingresos[[#Totals],[Columna10]]-Egresos[[#Totals],[Columna10]]</f>
+        <v>12056087.779999999</v>
+      </c>
+      <c r="M31" s="10">
+        <f>M5+Ingresos[[#Totals],[Columna11]]-Egresos[[#Totals],[Columna11]]</f>
+        <v>10343319.779999999</v>
+      </c>
+      <c r="N31" s="10">
+        <f>N5+Ingresos[[#Totals],[Columna12]]-Egresos[[#Totals],[Columna12]]</f>
+        <v>8630551.7799999993</v>
+      </c>
+      <c r="O31" s="10"/>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B33" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+    </row>
+    <row r="34" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-      <c r="M28">
-        <v>0</v>
-      </c>
-      <c r="N28">
-        <v>0</v>
-      </c>
-      <c r="O28">
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
         <f>SUM(Financiamiento[[#This Row],[Columna1]:[Columna12]])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:15" ht="15" x14ac:dyDescent="0.25">
-      <c r="B29" s="8" t="s">
+    <row r="35" spans="2:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="B35" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <f>SUM(Financiamiento[[#This Row],[Columna1]:[Columna12]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="M29">
-        <v>0</v>
-      </c>
-      <c r="N29">
-        <v>0</v>
-      </c>
-      <c r="O29">
-        <f>SUM(Financiamiento[[#This Row],[Columna1]:[Columna12]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C30" s="1">
+      <c r="C36" s="1">
         <f>SUM(Financiamiento[Columna1])</f>
         <v>0</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D36" s="1">
         <f>SUM(Financiamiento[Columna2])</f>
         <v>0</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E36" s="1">
         <f>SUM(Financiamiento[Columna3])</f>
         <v>0</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F36" s="1">
         <f>SUM(Financiamiento[Columna4])</f>
         <v>0</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G36" s="1">
         <f>SUM(Financiamiento[Columna5])</f>
         <v>0</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H36" s="1">
         <f>SUM(Financiamiento[Columna6])</f>
         <v>0</v>
       </c>
-      <c r="I30" s="1">
+      <c r="I36" s="1">
         <f>SUM(Financiamiento[Columna7])</f>
         <v>0</v>
       </c>
-      <c r="J30" s="1">
+      <c r="J36" s="1">
         <f>SUM(Financiamiento[Columna8])</f>
         <v>0</v>
       </c>
-      <c r="K30" s="1">
+      <c r="K36" s="1">
         <f>SUM(Financiamiento[Columna9])</f>
         <v>0</v>
       </c>
-      <c r="L30" s="1">
+      <c r="L36" s="1">
         <f>SUM(Financiamiento[Columna10])</f>
         <v>0</v>
       </c>
-      <c r="M30" s="1">
+      <c r="M36" s="1">
         <f>SUM(Financiamiento[Columna11])</f>
         <v>0</v>
       </c>
-      <c r="N30" s="1">
+      <c r="N36" s="1">
         <f>SUM(Financiamiento[Columna12])</f>
         <v>0</v>
       </c>
-      <c r="O30" s="1">
+      <c r="O36" s="1">
         <f>SUM(Financiamiento[#Totals])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="9" t="s">
+    <row r="38" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="10">
-        <f>C25-Financiamiento[[#Totals],[Columna1]]</f>
-        <v>1850000</v>
-      </c>
-      <c r="D32" s="10">
-        <f>D25-Financiamiento[[#Totals],[Columna2]]</f>
-        <v>2280000</v>
-      </c>
-      <c r="E32" s="10">
-        <f>E25-Financiamiento[[#Totals],[Columna3]]</f>
-        <v>2110000</v>
-      </c>
-      <c r="F32" s="10">
-        <f>F25-Financiamiento[[#Totals],[Columna4]]</f>
-        <v>2420000</v>
-      </c>
-      <c r="G32" s="10">
-        <f>G25-Financiamiento[[#Totals],[Columna5]]</f>
-        <v>2160000</v>
-      </c>
-      <c r="H32" s="10">
-        <f>H25-Financiamiento[[#Totals],[Columna6]]</f>
-        <v>1690000</v>
-      </c>
-      <c r="I32" s="10">
-        <f>I25-Financiamiento[[#Totals],[Columna7]]</f>
-        <v>1690000</v>
-      </c>
-      <c r="J32" s="10">
-        <f>J25-Financiamiento[[#Totals],[Columna8]]</f>
-        <v>1690000</v>
-      </c>
-      <c r="K32" s="10">
-        <f>K25-Financiamiento[[#Totals],[Columna9]]</f>
-        <v>1690000</v>
-      </c>
-      <c r="L32" s="10">
-        <f>L25-Financiamiento[[#Totals],[Columna10]]</f>
-        <v>1690000</v>
-      </c>
-      <c r="M32" s="10">
-        <f>M25-Financiamiento[[#Totals],[Columna11]]</f>
-        <v>1690000</v>
-      </c>
-      <c r="N32" s="10">
-        <f>N25-Financiamiento[[#Totals],[Columna12]]</f>
-        <v>1690000</v>
-      </c>
-      <c r="O32" s="10"/>
+      <c r="C38" s="10">
+        <f>C31-Financiamiento[[#Totals],[Columna1]]</f>
+        <v>6280237</v>
+      </c>
+      <c r="D38" s="10">
+        <f>D31-Financiamiento[[#Totals],[Columna2]]</f>
+        <v>5448343.3899999997</v>
+      </c>
+      <c r="E38" s="10">
+        <f>E31-Financiamiento[[#Totals],[Columna3]]</f>
+        <v>3800974.3899999997</v>
+      </c>
+      <c r="F38" s="10">
+        <f>F31-Financiamiento[[#Totals],[Columna4]]</f>
+        <v>2812084.78</v>
+      </c>
+      <c r="G38" s="10">
+        <f>G31-Financiamiento[[#Totals],[Columna5]]</f>
+        <v>11018518.779999999</v>
+      </c>
+      <c r="H38" s="10">
+        <f>H31-Financiamiento[[#Totals],[Columna6]]</f>
+        <v>8907159.7799999993</v>
+      </c>
+      <c r="I38" s="10">
+        <f>I31-Financiamiento[[#Totals],[Columna7]]</f>
+        <v>7194391.7799999993</v>
+      </c>
+      <c r="J38" s="10">
+        <f>J31-Financiamiento[[#Totals],[Columna8]]</f>
+        <v>5481623.7799999993</v>
+      </c>
+      <c r="K38" s="10">
+        <f>K31-Financiamiento[[#Totals],[Columna9]]</f>
+        <v>13768855.779999999</v>
+      </c>
+      <c r="L38" s="10">
+        <f>L31-Financiamiento[[#Totals],[Columna10]]</f>
+        <v>12056087.779999999</v>
+      </c>
+      <c r="M38" s="10">
+        <f>M31-Financiamiento[[#Totals],[Columna11]]</f>
+        <v>10343319.779999999</v>
+      </c>
+      <c r="N38" s="10">
+        <f>N31-Financiamiento[[#Totals],[Columna12]]</f>
+        <v>8630551.7799999993</v>
+      </c>
+      <c r="O38" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2609,82 +3057,38 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
         <x14:sparklineGroup displayEmptyCellsAs="gap">
-          <x14:colorSeries theme="4" tint="-0.499984740745262"/>
-          <x14:colorNegative theme="5"/>
+          <x14:colorSeries theme="5"/>
+          <x14:colorNegative theme="6"/>
           <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers theme="4" tint="-0.499984740745262"/>
-          <x14:colorFirst theme="4" tint="0.39997558519241921"/>
-          <x14:colorLast theme="4" tint="0.39997558519241921"/>
-          <x14:colorHigh theme="4"/>
-          <x14:colorLow theme="4"/>
+          <x14:colorMarkers theme="5" tint="-0.249977111117893"/>
+          <x14:colorFirst theme="5" tint="-0.249977111117893"/>
+          <x14:colorLast theme="5" tint="-0.249977111117893"/>
+          <x14:colorHigh theme="5" tint="-0.249977111117893"/>
+          <x14:colorLow theme="5" tint="-0.249977111117893"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Flujo de caja'!C32:N32</xm:f>
-              <xm:sqref>P32</xm:sqref>
+              <xm:f>'Flujo de caja'!C17:N17</xm:f>
+              <xm:sqref>P17</xm:sqref>
             </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap">
-          <x14:colorSeries theme="9" tint="-0.249977111117893"/>
-          <x14:colorNegative theme="4"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers theme="4" tint="-0.249977111117893"/>
-          <x14:colorFirst theme="4" tint="-0.249977111117893"/>
-          <x14:colorLast theme="4" tint="-0.249977111117893"/>
-          <x14:colorHigh theme="4" tint="-0.249977111117893"/>
-          <x14:colorLow theme="4" tint="-0.249977111117893"/>
-          <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Flujo de caja'!C30:N30</xm:f>
-              <xm:sqref>P30</xm:sqref>
+              <xm:f>'Flujo de caja'!C18:N18</xm:f>
+              <xm:sqref>P18</xm:sqref>
             </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap">
-          <x14:colorSeries theme="9" tint="-0.249977111117893"/>
-          <x14:colorNegative theme="4"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers theme="4" tint="-0.249977111117893"/>
-          <x14:colorFirst theme="4" tint="-0.249977111117893"/>
-          <x14:colorLast theme="4" tint="-0.249977111117893"/>
-          <x14:colorHigh theme="4" tint="-0.249977111117893"/>
-          <x14:colorLow theme="4" tint="-0.249977111117893"/>
-          <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Flujo de caja'!C29:N29</xm:f>
-              <xm:sqref>P29</xm:sqref>
+              <xm:f>'Flujo de caja'!C19:N19</xm:f>
+              <xm:sqref>P19</xm:sqref>
             </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap">
-          <x14:colorSeries theme="9" tint="-0.249977111117893"/>
-          <x14:colorNegative theme="4"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers theme="4" tint="-0.249977111117893"/>
-          <x14:colorFirst theme="4" tint="-0.249977111117893"/>
-          <x14:colorLast theme="4" tint="-0.249977111117893"/>
-          <x14:colorHigh theme="4" tint="-0.249977111117893"/>
-          <x14:colorLow theme="4" tint="-0.249977111117893"/>
-          <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Flujo de caja'!C28:N28</xm:f>
-              <xm:sqref>P28</xm:sqref>
+              <xm:f>'Flujo de caja'!C20:N20</xm:f>
+              <xm:sqref>P20</xm:sqref>
             </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap">
-          <x14:colorSeries theme="4" tint="-0.499984740745262"/>
-          <x14:colorNegative theme="5"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers theme="4" tint="-0.499984740745262"/>
-          <x14:colorFirst theme="4" tint="0.39997558519241921"/>
-          <x14:colorLast theme="4" tint="0.39997558519241921"/>
-          <x14:colorHigh theme="4"/>
-          <x14:colorLow theme="4"/>
-          <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Flujo de caja'!C25:N25</xm:f>
-              <xm:sqref>P25</xm:sqref>
+              <xm:f>'Flujo de caja'!C21:N21</xm:f>
+              <xm:sqref>P21</xm:sqref>
+            </x14:sparkline>
+            <x14:sparkline>
+              <xm:f>'Flujo de caja'!C22:N22</xm:f>
+              <xm:sqref>P22</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -2715,8 +3119,8 @@
           <x14:colorLow theme="5" tint="-0.249977111117893"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Flujo de caja'!C22:N22</xm:f>
-              <xm:sqref>P22</xm:sqref>
+              <xm:f>'Flujo de caja'!C24:N24</xm:f>
+              <xm:sqref>P24</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -2731,8 +3135,8 @@
           <x14:colorLow theme="5" tint="-0.249977111117893"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Flujo de caja'!C21:N21</xm:f>
-              <xm:sqref>P21</xm:sqref>
+              <xm:f>'Flujo de caja'!C25:N25</xm:f>
+              <xm:sqref>P25</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -2747,8 +3151,8 @@
           <x14:colorLow theme="5" tint="-0.249977111117893"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Flujo de caja'!C20:N20</xm:f>
-              <xm:sqref>P20</xm:sqref>
+              <xm:f>'Flujo de caja'!C26:N26</xm:f>
+              <xm:sqref>P26</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -2763,8 +3167,8 @@
           <x14:colorLow theme="5" tint="-0.249977111117893"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Flujo de caja'!C19:N19</xm:f>
-              <xm:sqref>P19</xm:sqref>
+              <xm:f>'Flujo de caja'!C27:N27</xm:f>
+              <xm:sqref>P27</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -2779,8 +3183,8 @@
           <x14:colorLow theme="5" tint="-0.249977111117893"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Flujo de caja'!C18:N18</xm:f>
-              <xm:sqref>P18</xm:sqref>
+              <xm:f>'Flujo de caja'!C28:N28</xm:f>
+              <xm:sqref>P28</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -2795,24 +3199,88 @@
           <x14:colorLow theme="5" tint="-0.249977111117893"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Flujo de caja'!C17:N17</xm:f>
-              <xm:sqref>P17</xm:sqref>
+              <xm:f>'Flujo de caja'!C29:N29</xm:f>
+              <xm:sqref>P29</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
         <x14:sparklineGroup displayEmptyCellsAs="gap">
-          <x14:colorSeries theme="5"/>
-          <x14:colorNegative theme="6"/>
+          <x14:colorSeries theme="4" tint="-0.499984740745262"/>
+          <x14:colorNegative theme="5"/>
           <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers theme="5" tint="-0.249977111117893"/>
-          <x14:colorFirst theme="5" tint="-0.249977111117893"/>
-          <x14:colorLast theme="5" tint="-0.249977111117893"/>
-          <x14:colorHigh theme="5" tint="-0.249977111117893"/>
-          <x14:colorLow theme="5" tint="-0.249977111117893"/>
+          <x14:colorMarkers theme="4" tint="-0.499984740745262"/>
+          <x14:colorFirst theme="4" tint="0.39997558519241921"/>
+          <x14:colorLast theme="4" tint="0.39997558519241921"/>
+          <x14:colorHigh theme="4"/>
+          <x14:colorLow theme="4"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Flujo de caja'!C16:N16</xm:f>
-              <xm:sqref>P16</xm:sqref>
+              <xm:f>'Flujo de caja'!C31:N31</xm:f>
+              <xm:sqref>P31</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap">
+          <x14:colorSeries theme="9" tint="-0.249977111117893"/>
+          <x14:colorNegative theme="4"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers theme="4" tint="-0.249977111117893"/>
+          <x14:colorFirst theme="4" tint="-0.249977111117893"/>
+          <x14:colorLast theme="4" tint="-0.249977111117893"/>
+          <x14:colorHigh theme="4" tint="-0.249977111117893"/>
+          <x14:colorLow theme="4" tint="-0.249977111117893"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Flujo de caja'!C34:N34</xm:f>
+              <xm:sqref>P34</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap">
+          <x14:colorSeries theme="9" tint="-0.249977111117893"/>
+          <x14:colorNegative theme="4"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers theme="4" tint="-0.249977111117893"/>
+          <x14:colorFirst theme="4" tint="-0.249977111117893"/>
+          <x14:colorLast theme="4" tint="-0.249977111117893"/>
+          <x14:colorHigh theme="4" tint="-0.249977111117893"/>
+          <x14:colorLow theme="4" tint="-0.249977111117893"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Flujo de caja'!C35:N35</xm:f>
+              <xm:sqref>P35</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap">
+          <x14:colorSeries theme="9" tint="-0.249977111117893"/>
+          <x14:colorNegative theme="4"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers theme="4" tint="-0.249977111117893"/>
+          <x14:colorFirst theme="4" tint="-0.249977111117893"/>
+          <x14:colorLast theme="4" tint="-0.249977111117893"/>
+          <x14:colorHigh theme="4" tint="-0.249977111117893"/>
+          <x14:colorLow theme="4" tint="-0.249977111117893"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Flujo de caja'!C36:N36</xm:f>
+              <xm:sqref>P36</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap">
+          <x14:colorSeries theme="4" tint="-0.499984740745262"/>
+          <x14:colorNegative theme="5"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers theme="4" tint="-0.499984740745262"/>
+          <x14:colorFirst theme="4" tint="0.39997558519241921"/>
+          <x14:colorLast theme="4" tint="0.39997558519241921"/>
+          <x14:colorHigh theme="4"/>
+          <x14:colorLow theme="4"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Flujo de caja'!C38:N38</xm:f>
+              <xm:sqref>P38</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -2912,8 +3380,184 @@
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
+        <x14:sparklineGroup displayEmptyCellsAs="gap">
+          <x14:colorSeries theme="5"/>
+          <x14:colorNegative theme="6"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers theme="5" tint="-0.249977111117893"/>
+          <x14:colorFirst theme="5" tint="-0.249977111117893"/>
+          <x14:colorLast theme="5" tint="-0.249977111117893"/>
+          <x14:colorHigh theme="5" tint="-0.249977111117893"/>
+          <x14:colorLow theme="5" tint="-0.249977111117893"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Flujo de caja'!C16:N16</xm:f>
+              <xm:sqref>P16</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
       </x14:sparklineGroups>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="14"/>
+    <col min="3" max="3" width="11.42578125" style="17"/>
+    <col min="4" max="4" width="11.42578125" style="14"/>
+    <col min="5" max="5" width="10.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="15">
+        <v>2018</v>
+      </c>
+      <c r="C1" s="16">
+        <v>2019</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+    </row>
+    <row r="2" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="13">
+        <v>781242</v>
+      </c>
+      <c r="C2" s="13">
+        <v>828116</v>
+      </c>
+      <c r="E2" s="13">
+        <f>B2*B3</f>
+        <v>66405.570000000007</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="19">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="C3" s="19">
+        <v>8.5000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="18">
+        <v>0.12</v>
+      </c>
+      <c r="C4" s="18">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="21">
+        <v>0.02</v>
+      </c>
+      <c r="C5" s="21">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="21">
+        <v>0.03</v>
+      </c>
+      <c r="C6" s="21">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="21">
+        <v>0.04</v>
+      </c>
+      <c r="C7" s="21">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="20">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="C8" s="20">
+        <v>8.3299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="21">
+        <v>0.01</v>
+      </c>
+      <c r="C9" s="18">
+        <f>1%</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="20">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="C10" s="20">
+        <v>8.3299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="22">
+        <v>4.1700000000000001E-2</v>
+      </c>
+      <c r="C11" s="23">
+        <v>4.1700000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="22">
+        <v>5.2199999999999998E-3</v>
+      </c>
+      <c r="C12" s="22">
+        <v>5.2199999999999998E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>